<commit_message>
saved new annual PDO data as csv
</commit_message>
<xml_diff>
--- a/data/Environmental/ENSO.xlsx
+++ b/data/Environmental/ENSO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracehenry/Documents/GitHub/CSIA_lab_work/data/environmental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21622F2E-454B-6445-8BFB-9B095BCEFAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E69704-7CCE-8349-9A14-AE294C3930DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15940" xr2:uid="{AA97590B-D8AE-6643-9B1E-9841361F977D}"/>
   </bookViews>
@@ -40,40 +40,40 @@
     <t>Year</t>
   </si>
   <si>
-    <t xml:space="preserve">January </t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t xml:space="preserve">April </t>
-  </si>
-  <si>
     <t>May</t>
   </si>
   <si>
-    <t>June</t>
+    <t>Jan</t>
   </si>
   <si>
-    <t>July</t>
+    <t>Feb</t>
   </si>
   <si>
-    <t>August</t>
+    <t>Mar</t>
   </si>
   <si>
-    <t xml:space="preserve">September </t>
+    <t>Apr</t>
   </si>
   <si>
-    <t>October</t>
+    <t>Jun</t>
   </si>
   <si>
-    <t>November</t>
+    <t>Jul</t>
   </si>
   <si>
-    <t>December</t>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:M155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A155"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -446,19 +446,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" t="s">
         <v>6</v>

</xml_diff>